<commit_message>
Add GIS file and last network data excel file
</commit_message>
<xml_diff>
--- a/EBSD_Tutorial/data/EBSD_Tutorial_Data.xlsx
+++ b/EBSD_Tutorial/data/EBSD_Tutorial_Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Data\demos\data\EBSD_Tutorial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\Apps\demos\data\EBSD_Tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="14430" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="14430" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="network" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="187">
   <si>
     <t>Name</t>
   </si>
@@ -468,69 +468,27 @@
     <t>1e6 m^3</t>
   </si>
   <si>
-    <t>225.0000000000</t>
-  </si>
-  <si>
-    <t>443.0000000000</t>
-  </si>
-  <si>
     <t>optSou</t>
   </si>
   <si>
     <t>optional future node</t>
   </si>
   <si>
-    <t>176.0000000000</t>
-  </si>
-  <si>
-    <t>123.0000000000</t>
-  </si>
-  <si>
     <t>dem</t>
   </si>
   <si>
     <t>demand node</t>
   </si>
   <si>
-    <t>336.0000000000</t>
-  </si>
-  <si>
-    <t>359.0000000000</t>
-  </si>
-  <si>
-    <t>25.0000000000</t>
-  </si>
-  <si>
-    <t>57.0000000000</t>
-  </si>
-  <si>
-    <t>116.0000000000</t>
-  </si>
-  <si>
-    <t>13.0000000000</t>
-  </si>
-  <si>
     <t>exDO</t>
   </si>
   <si>
     <t>Existing node</t>
   </si>
   <si>
-    <t>427.0000000000</t>
-  </si>
-  <si>
-    <t>425.0000000000</t>
-  </si>
-  <si>
     <t>junc1</t>
   </si>
   <si>
-    <t>241.0000000000</t>
-  </si>
-  <si>
-    <t>271.0000000000</t>
-  </si>
-  <si>
     <t>junct</t>
   </si>
   <si>
@@ -540,18 +498,6 @@
     <t>junc2</t>
   </si>
   <si>
-    <t>273.0000000000</t>
-  </si>
-  <si>
-    <t>183.0000000000</t>
-  </si>
-  <si>
-    <t>489.0000000000</t>
-  </si>
-  <si>
-    <t>332.0000000000</t>
-  </si>
-  <si>
     <t>link</t>
   </si>
   <si>
@@ -622,6 +568,42 @@
   </si>
   <si>
     <t>Text</t>
+  </si>
+  <si>
+    <t>annualised capital and operating cost of sources&amp;links [-]</t>
+  </si>
+  <si>
+    <t>Activation for optional source during period t [-]</t>
+  </si>
+  <si>
+    <t>Activitation of link optilnal during period t [-]</t>
+  </si>
+  <si>
+    <t>Flow from node i to j during year t [1e6 m^3 mon^-1]</t>
+  </si>
+  <si>
+    <t>Supply from source i during year t [1e6 m^3]</t>
+  </si>
+  <si>
+    <t>maximum capacity [Ml/d]</t>
+  </si>
+  <si>
+    <t>variable operating costs for sources [k£/t]</t>
+  </si>
+  <si>
+    <t>fixed operating costs for sources  [k£/t]</t>
+  </si>
+  <si>
+    <t>fixed operating costs for links [k£/t]</t>
+  </si>
+  <si>
+    <t>variable operating costs for links [k£/t]</t>
+  </si>
+  <si>
+    <t>demand required over a planning period of 25 years [Ml/d].</t>
+  </si>
+  <si>
+    <t>Capital cost [k£]</t>
   </si>
 </sst>
 </file>
@@ -666,9 +648,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -952,7 +937,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1070,7 +1057,7 @@
         <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1078,7 +1065,7 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1145,34 +1132,34 @@
         <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -1180,34 +1167,34 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="D2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="F2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="H2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="J2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="L2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="N2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="P2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="R2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="T2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -1373,34 +1360,34 @@
         <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -1408,34 +1395,34 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="D2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="F2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="H2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="J2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="L2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="N2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="P2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="R2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="T2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -1601,34 +1588,34 @@
         <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -1636,34 +1623,34 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="D2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="F2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="H2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="J2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="L2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="N2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="P2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="R2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="T2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -1829,34 +1816,34 @@
         <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -1864,34 +1851,34 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="D2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="F2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="H2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="J2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="L2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="N2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="P2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="R2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="T2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -3027,12 +3014,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -3113,14 +3103,14 @@
       <c r="A3" t="s">
         <v>50</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>161874</v>
+      </c>
+      <c r="C3">
+        <v>6820509</v>
+      </c>
+      <c r="D3" t="s">
         <v>141</v>
-      </c>
-      <c r="C3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D3" t="s">
-        <v>143</v>
       </c>
       <c r="E3" s="1">
         <v>9500</v>
@@ -3138,61 +3128,61 @@
         <v>63</v>
       </c>
       <c r="M3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>106</v>
       </c>
-      <c r="B4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C4" t="s">
-        <v>146</v>
+      <c r="B4">
+        <v>88039</v>
+      </c>
+      <c r="C4">
+        <v>6921808</v>
       </c>
       <c r="D4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>21</v>
       </c>
       <c r="M4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>134</v>
       </c>
-      <c r="B5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C5" t="s">
-        <v>150</v>
+      <c r="B5">
+        <v>128778</v>
+      </c>
+      <c r="C5">
+        <v>6871885</v>
       </c>
       <c r="D5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="M5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>135</v>
       </c>
-      <c r="B6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C6" t="s">
-        <v>152</v>
+      <c r="B6">
+        <v>41012</v>
+      </c>
+      <c r="C6">
+        <v>6945406</v>
       </c>
       <c r="D6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E6" s="1">
         <v>27000</v>
@@ -3210,21 +3200,21 @@
         <v>225</v>
       </c>
       <c r="M6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>136</v>
       </c>
-      <c r="B7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C7" t="s">
-        <v>154</v>
+      <c r="B7">
+        <v>62684</v>
+      </c>
+      <c r="C7">
+        <v>6957628</v>
       </c>
       <c r="D7" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="F7" s="1">
         <v>50</v>
@@ -3239,21 +3229,21 @@
         <v>0.09</v>
       </c>
       <c r="M7" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>137</v>
       </c>
-      <c r="B8" t="s">
-        <v>157</v>
-      </c>
-      <c r="C8" t="s">
-        <v>158</v>
+      <c r="B8">
+        <v>173316</v>
+      </c>
+      <c r="C8">
+        <v>6846603</v>
       </c>
       <c r="D8" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="F8" s="1">
         <v>50</v>
@@ -3268,55 +3258,55 @@
         <v>0.11</v>
       </c>
       <c r="M8" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>159</v>
-      </c>
-      <c r="B9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C9" t="s">
-        <v>161</v>
+        <v>147</v>
+      </c>
+      <c r="B9">
+        <v>88087</v>
+      </c>
+      <c r="C9">
+        <v>6885380</v>
       </c>
       <c r="D9" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="M9" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>164</v>
-      </c>
-      <c r="B10" t="s">
-        <v>165</v>
-      </c>
-      <c r="C10" t="s">
-        <v>166</v>
+        <v>150</v>
+      </c>
+      <c r="B10">
+        <v>121098</v>
+      </c>
+      <c r="C10">
+        <v>6909129</v>
       </c>
       <c r="D10" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="M10" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>138</v>
       </c>
-      <c r="B11" t="s">
-        <v>167</v>
-      </c>
-      <c r="C11" t="s">
-        <v>168</v>
+      <c r="B11">
+        <v>185751</v>
+      </c>
+      <c r="C11">
+        <v>6873651</v>
       </c>
       <c r="D11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E11" s="1">
         <v>21000</v>
@@ -3334,7 +3324,7 @@
         <v>250</v>
       </c>
       <c r="M11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3476,8 +3466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3500,10 +3490,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="C1" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="D1" t="s">
         <v>34</v>
@@ -3561,7 +3551,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>50</v>
@@ -3570,7 +3560,7 @@
         <v>134</v>
       </c>
       <c r="D3" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="E3" s="1">
         <v>4</v>
@@ -3585,12 +3575,12 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>106</v>
@@ -3599,7 +3589,7 @@
         <v>134</v>
       </c>
       <c r="D4" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="E4" s="1">
         <v>14</v>
@@ -3620,21 +3610,21 @@
         <v>9000</v>
       </c>
       <c r="M4" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D5" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
@@ -3649,21 +3639,21 @@
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="D6" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="E6" s="1">
         <v>14</v>
@@ -3681,12 +3671,12 @@
         <v>19000</v>
       </c>
       <c r="M6" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>135</v>
@@ -3695,7 +3685,7 @@
         <v>106</v>
       </c>
       <c r="D7" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="E7" s="1">
         <v>6</v>
@@ -3710,12 +3700,12 @@
         <v>0</v>
       </c>
       <c r="M7" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>136</v>
@@ -3724,7 +3714,7 @@
         <v>106</v>
       </c>
       <c r="D8" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="E8" s="1">
         <v>50</v>
@@ -3739,12 +3729,12 @@
         <v>0</v>
       </c>
       <c r="M8" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>137</v>
@@ -3753,7 +3743,7 @@
         <v>134</v>
       </c>
       <c r="D9" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="E9" s="1">
         <v>50</v>
@@ -3768,21 +3758,21 @@
         <v>0</v>
       </c>
       <c r="M9" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>134</v>
       </c>
       <c r="D10" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="E10" s="1">
         <v>2</v>
@@ -3797,21 +3787,21 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="M10" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>134</v>
       </c>
       <c r="D11" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="E11" s="1">
         <v>14</v>
@@ -3829,12 +3819,12 @@
         <v>0</v>
       </c>
       <c r="M11" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>138</v>
@@ -3843,7 +3833,7 @@
         <v>134</v>
       </c>
       <c r="D12" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="E12" s="1">
         <v>4</v>
@@ -3858,7 +3848,7 @@
         <v>0</v>
       </c>
       <c r="M12" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -3990,7 +3980,7 @@
         <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -4002,14 +3992,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -4058,6 +4050,9 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
+      <c r="D4" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -4067,7 +4062,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4078,7 +4076,10 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4091,6 +4092,9 @@
       <c r="C7" t="s">
         <v>6</v>
       </c>
+      <c r="D7" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -4102,6 +4106,9 @@
       <c r="C8" t="s">
         <v>6</v>
       </c>
+      <c r="D8" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -4113,6 +4120,9 @@
       <c r="C9" t="s">
         <v>6</v>
       </c>
+      <c r="D9" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -4124,6 +4134,9 @@
       <c r="C10" t="s">
         <v>6</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -4144,7 +4157,10 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -4157,6 +4173,9 @@
       <c r="C13" t="s">
         <v>6</v>
       </c>
+      <c r="D13" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -4166,7 +4185,10 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -4179,6 +4201,9 @@
       <c r="C15" t="s">
         <v>6</v>
       </c>
+      <c r="D15" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -4262,6 +4287,9 @@
       <c r="C22" t="s">
         <v>32</v>
       </c>
+      <c r="D22" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -4276,6 +4304,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4298,7 +4327,7 @@
         <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -4346,10 +4375,10 @@
         <v>137</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>138</v>
@@ -4360,31 +4389,31 @@
         <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C2" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="F2" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="G2" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="H2" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="I2" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="J2" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -4392,22 +4421,22 @@
         <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C3" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="D3" t="s">
         <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="F3" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="G3" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="H3" t="s">
         <v>41</v>
@@ -4416,7 +4445,7 @@
         <v>41</v>
       </c>
       <c r="J3" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -4424,31 +4453,31 @@
         <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C4" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="D4" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="E4" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="F4" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="G4" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="H4" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="I4" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="J4" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -4456,31 +4485,31 @@
         <v>135</v>
       </c>
       <c r="B5" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C5" t="s">
         <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="E5" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="F5" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="G5" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="H5" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="I5" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="J5" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -4488,31 +4517,31 @@
         <v>136</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C6" t="s">
         <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="E6" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="F6" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="G6" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="H6" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="I6" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="J6" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -4520,95 +4549,95 @@
         <v>137</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="D7" t="s">
         <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="F7" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="G7" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="H7" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="I7" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="J7" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="B8" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C8" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="D8" t="s">
         <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="F8" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="G8" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="H8" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="I8" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="J8" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="B9" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C9" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="D9" t="s">
         <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="F9" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="G9" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="H9" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="I9" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="J9" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -4616,31 +4645,31 @@
         <v>138</v>
       </c>
       <c r="B10" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C10" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="D10" t="s">
         <v>41</v>
       </c>
       <c r="E10" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="F10" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="G10" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="H10" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="I10" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="J10" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -4690,13 +4719,13 @@
         <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -4704,13 +4733,13 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="D2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="F2" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>